<commit_message>
feat: updated and fixed after critique.
added datasets
added annotation to suicide_comparison chart
</commit_message>
<xml_diff>
--- a/datasets/ACT_mental_health.xlsx
+++ b/datasets/ACT_mental_health.xlsx
@@ -1,50 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\corp\absdfs\applications\SuperSTAR2\C447\Tables\Development\Mental Health and Wellbeing (Survey of)\Pooled (2020-22)\DATACUBES\Tables ACT\Completed Accessible table\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E88823B-4336-428F-B781-830CF20E3483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="14580" yWindow="-16395" windowWidth="29040" windowHeight="15840" xr2:uid="{7D117995-1A8A-4D69-A5E9-331272F06E4F}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Contents" sheetId="1" r:id="rId1"/>
-    <sheet name="Table 1.1 Estimates" sheetId="2" r:id="rId2"/>
-    <sheet name="Table 1.2 RSEs" sheetId="3" r:id="rId3"/>
-    <sheet name="Table 1.3 Proportions" sheetId="4" r:id="rId4"/>
-    <sheet name="Table 1.4 MoEs" sheetId="5" r:id="rId5"/>
-  </sheets>
-  <definedNames>
-    <definedName name="_AMO_UniqueIdentifier" hidden="1">"'3a04a3ef-8af1-40be-945d-6079cf21e0d2'"</definedName>
-    <definedName name="This_tab_has_one_table_with_95_percent_Margin_of_Error_of_proportion_of_Persons_16–85_years_in_Australian_Capital_Territory_Lifetime_and_12_month_mental_disorder_groups._It_ranges_from_cell_A1_to_B35.">'Table 1.4 MoEs'!$A$1:$B$35</definedName>
-    <definedName name="This_tab_has_one_table_with_Estimate_of_Persons_16–85_years_in_Australian_Capital_Territory_Lifetime_and_12_month_mental_disorder_groups._It_ranges_from_cell_A1_to_B36.">'Table 1.1 Estimates'!$A$1:$B$36</definedName>
-    <definedName name="This_tab_has_one_table_with_Proportion_of_Persons_16–85_years_in_Australian_Capital_Territory_Lifetime_and_12_month_mental_disorder_groups._It_ranges_from_cell_A1_to_B35.">'Table 1.3 Proportions'!$A$1:$B$35</definedName>
-    <definedName name="This_tab_has_one_table_with_Relative_Standard_Error_of_estimate_of_Persons_16–85_years_in_Australian_Capital_Territory_Lifetime_and_12_month_mental_disorder_groups._It_ranges_from_cell_A1_to_B35.">'Table 1.2 RSEs'!$A$1:$B$35</definedName>
-    <definedName name="This_tab_outlines_the_contents_of_the_datacube_for_the_Australian_Capital_Territory._It_ranges_from_cell_A1_to_B17.">Contents!$A$1:$B$17</definedName>
-  </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
-</workbook>
+<ns0:workbook xmlns:ns0="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ns1="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:ns2="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:ns3="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:ns4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:ns5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:ns6="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:ns7="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ns8="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:ns9="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" ns1:Ignorable="x15 xr xr6 xr10 xr2">
+  <ns0:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <ns0:workbookPr defaultThemeVersion="166925"/>
+  <ns1:AlternateContent>
+    <ns1:Choice Requires="x15">
+      <ns2:absPath url="\\corp\absdfs\applications\SuperSTAR2\C447\Tables\Development\Mental Health and Wellbeing (Survey of)\Pooled (2020-22)\DATACUBES\Tables ACT\Completed Accessible table\"/>
+    </ns1:Choice>
+  </ns1:AlternateContent>
+  <ns3:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E88823B-4336-428F-B781-830CF20E3483}" ns4:coauthVersionLast="47" ns4:coauthVersionMax="47" ns5:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <ns0:bookViews>
+    <ns0:workbookView xWindow="14580" yWindow="-16395" windowWidth="29040" windowHeight="15840" ns6:uid="{7D117995-1A8A-4D69-A5E9-331272F06E4F}"/>
+  </ns0:bookViews>
+  <ns0:sheets>
+    <ns0:sheet name="Contents" sheetId="1" ns7:id="rId1"/>
+    <ns0:sheet name="Table 1.1 Estimates" sheetId="2" ns7:id="rId2"/>
+    <ns0:sheet name="Table 1.3 Proportions" sheetId="4" ns7:id="rId4"/>
+  </ns0:sheets>
+  <ns0:definedNames>
+    <ns0:definedName name="_AMO_UniqueIdentifier" hidden="1">"'3a04a3ef-8af1-40be-945d-6079cf21e0d2'"</ns0:definedName>
+    <ns0:definedName name="This_tab_has_one_table_with_95_percent_Margin_of_Error_of_proportion_of_Persons_16–85_years_in_Australian_Capital_Territory_Lifetime_and_12_month_mental_disorder_groups._It_ranges_from_cell_A1_to_B35.">'Table 1.4 MoEs'!$A$1:$B$35</ns0:definedName>
+    <ns0:definedName name="This_tab_has_one_table_with_Estimate_of_Persons_16–85_years_in_Australian_Capital_Territory_Lifetime_and_12_month_mental_disorder_groups._It_ranges_from_cell_A1_to_B36.">'Table 1.1 Estimates'!$A$1:$B$36</ns0:definedName>
+    <ns0:definedName name="This_tab_has_one_table_with_Proportion_of_Persons_16–85_years_in_Australian_Capital_Territory_Lifetime_and_12_month_mental_disorder_groups._It_ranges_from_cell_A1_to_B35.">'Table 1.3 Proportions'!$A$1:$B$35</ns0:definedName>
+    <ns0:definedName name="This_tab_has_one_table_with_Relative_Standard_Error_of_estimate_of_Persons_16–85_years_in_Australian_Capital_Territory_Lifetime_and_12_month_mental_disorder_groups._It_ranges_from_cell_A1_to_B35.">'Table 1.2 RSEs'!$A$1:$B$35</ns0:definedName>
+    <ns0:definedName name="This_tab_outlines_the_contents_of_the_datacube_for_the_Australian_Capital_Territory._It_ranges_from_cell_A1_to_B17.">Contents!$A$1:$B$17</ns0:definedName>
+  </ns0:definedNames>
+  <ns0:calcPr calcId="191029"/>
+  <ns0:extLst>
+    <ns0:ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <ns8:workbookPr chartTrackingRefBase="1"/>
+    </ns0:ext>
+    <ns0:ext uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <ns9:calcFeatures>
+        <ns9:feature name="microsoft.com:RD"/>
+        <ns9:feature name="microsoft.com:Single"/>
+        <ns9:feature name="microsoft.com:FV"/>
+        <ns9:feature name="microsoft.com:CNMTM"/>
+        <ns9:feature name="microsoft.com:LET_WF"/>
+        <ns9:feature name="microsoft.com:LAMBDA_WF"/>
+        <ns9:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </ns9:calcFeatures>
+    </ns0:ext>
+  </ns0:extLst>
+</ns0:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>